<commit_message>
partially the fake data creation was made
</commit_message>
<xml_diff>
--- a/CRUDCreateCode/data/input/models/CustomerB2B.xlsx
+++ b/CRUDCreateCode/data/input/models/CustomerB2B.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tkax/dev/aimonetize/Backend/DjangoBasic/CRUDCreateCode/data/input/models/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6C37245-1D55-FE41-A1F6-B1D9439541C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{622050D1-1926-6E41-B91F-15707BA731B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10060" yWindow="2280" windowWidth="28000" windowHeight="18880" xr2:uid="{43DD2820-FE61-F645-B31F-194723807C3A}"/>
+    <workbookView xWindow="10020" yWindow="1600" windowWidth="28000" windowHeight="18880" xr2:uid="{43DD2820-FE61-F645-B31F-194723807C3A}"/>
   </bookViews>
   <sheets>
     <sheet name="model" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
     <sheet name="html" sheetId="5" r:id="rId11"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">model!$B$1:$Z$68</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">model!$B$1:$AB$68</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="589" uniqueCount="163">
   <si>
     <t>Variable</t>
   </si>
@@ -356,21 +356,6 @@
   </si>
   <si>
     <t>CustomerB2BAggregate_country</t>
-  </si>
-  <si>
-    <t xml:space="preserve">country </t>
-  </si>
-  <si>
-    <t xml:space="preserve">total_customers </t>
-  </si>
-  <si>
-    <t xml:space="preserve">total_annual_revenue </t>
-  </si>
-  <si>
-    <t xml:space="preserve">total_industries </t>
-  </si>
-  <si>
-    <t xml:space="preserve">total_company_size </t>
   </si>
   <si>
     <t>models.IntegerField(default=0)</t>
@@ -444,9 +429,6 @@
     <t>surname</t>
   </si>
   <si>
-    <t>firstname</t>
-  </si>
-  <si>
     <t>description</t>
   </si>
   <si>
@@ -525,6 +507,81 @@
   </si>
   <si>
     <t>models.PositiveIntegerField(blank=True,null=True,help_text="Number of employees")</t>
+  </si>
+  <si>
+    <t>total_customers</t>
+  </si>
+  <si>
+    <t>total_annual_revenue</t>
+  </si>
+  <si>
+    <t>total_industries</t>
+  </si>
+  <si>
+    <t>total_company_size</t>
+  </si>
+  <si>
+    <t>CustomerB2BGroup</t>
+  </si>
+  <si>
+    <t>text(max_nb_chars=200)</t>
+  </si>
+  <si>
+    <t>name()</t>
+  </si>
+  <si>
+    <t>email()</t>
+  </si>
+  <si>
+    <t>phone()</t>
+  </si>
+  <si>
+    <t>uri()</t>
+  </si>
+  <si>
+    <t>address()</t>
+  </si>
+  <si>
+    <t>city()</t>
+  </si>
+  <si>
+    <t>state()</t>
+  </si>
+  <si>
+    <t>zipcode()</t>
+  </si>
+  <si>
+    <t>counrtry()</t>
+  </si>
+  <si>
+    <t>user_name()</t>
+  </si>
+  <si>
+    <t>faker_type</t>
+  </si>
+  <si>
+    <t>integer</t>
+  </si>
+  <si>
+    <t>float</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>first_name</t>
+  </si>
+  <si>
+    <t>last_name()</t>
+  </si>
+  <si>
+    <t>fake.numerify(text='#########')</t>
+  </si>
+  <si>
+    <t>faker_function</t>
+  </si>
+  <si>
+    <t>char</t>
   </si>
 </sst>
 </file>
@@ -894,25 +951,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E15A4BF7-DFDE-D24F-85FE-657339D228CC}">
-  <dimension ref="A1:Z70"/>
+  <dimension ref="A1:AB70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B32" workbookViewId="0">
-      <selection activeCell="E61" sqref="E61"/>
+    <sheetView tabSelected="1" topLeftCell="B38" workbookViewId="0">
+      <selection activeCell="H61" sqref="H61:H67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18" customWidth="1"/>
     <col min="3" max="3" width="24.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="28.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="72.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="32.1640625" customWidth="1"/>
-    <col min="7" max="13" width="11.1640625" customWidth="1"/>
+    <col min="6" max="8" width="32.1640625" customWidth="1"/>
+    <col min="9" max="15" width="11.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -930,67 +988,73 @@
         <v>30</v>
       </c>
       <c r="G1" t="s">
+        <v>161</v>
+      </c>
+      <c r="H1" t="s">
+        <v>154</v>
+      </c>
+      <c r="I1" t="s">
         <v>13</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>17</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>21</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>18</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>19</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>15</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>16</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>8</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>9</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>10</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="S1" t="s">
         <v>11</v>
       </c>
-      <c r="R1" t="s">
+      <c r="T1" t="s">
         <v>20</v>
       </c>
-      <c r="S1" t="s">
+      <c r="U1" t="s">
         <v>27</v>
       </c>
-      <c r="T1" t="s">
+      <c r="V1" t="s">
         <v>28</v>
       </c>
-      <c r="U1" t="s">
+      <c r="W1" t="s">
         <v>25</v>
       </c>
-      <c r="V1" t="s">
+      <c r="X1" t="s">
         <v>26</v>
       </c>
-      <c r="W1" t="s">
+      <c r="Y1" t="s">
         <v>12</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Z1" t="s">
         <v>22</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AA1" t="s">
         <v>23</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AB1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>34</v>
       </c>
@@ -1009,20 +1073,26 @@
       <c r="F2" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="V2" s="2">
-        <v>1</v>
-      </c>
-      <c r="W2" s="2">
-        <v>1</v>
+      <c r="G2" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>162</v>
       </c>
       <c r="X2" s="2">
         <v>1</v>
       </c>
+      <c r="Y2" s="2">
+        <v>1</v>
+      </c>
       <c r="Z2" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AB2" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>34</v>
       </c>
@@ -1041,21 +1111,27 @@
       <c r="F3" t="s">
         <v>67</v>
       </c>
-      <c r="R3" s="2"/>
-      <c r="V3" s="2">
-        <v>1</v>
-      </c>
-      <c r="W3">
-        <v>1</v>
-      </c>
+      <c r="G3" t="s">
+        <v>145</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="T3" s="2"/>
       <c r="X3" s="2">
         <v>1</v>
       </c>
+      <c r="Y3">
+        <v>1</v>
+      </c>
       <c r="Z3" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AB3" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>34</v>
       </c>
@@ -1074,19 +1150,25 @@
       <c r="F4" t="s">
         <v>68</v>
       </c>
-      <c r="P4" s="2"/>
-      <c r="Q4" s="2"/>
-      <c r="V4" s="2">
-        <v>1</v>
-      </c>
+      <c r="G4" t="s">
+        <v>146</v>
+      </c>
+      <c r="H4" t="s">
+        <v>162</v>
+      </c>
+      <c r="R4" s="2"/>
+      <c r="S4" s="2"/>
       <c r="X4" s="2">
         <v>1</v>
       </c>
       <c r="Z4" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AB4" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>34</v>
       </c>
@@ -1105,8 +1187,11 @@
       <c r="F5" t="s">
         <v>69</v>
       </c>
-      <c r="V5" s="2">
-        <v>1</v>
+      <c r="G5" t="s">
+        <v>147</v>
+      </c>
+      <c r="H5" t="s">
+        <v>162</v>
       </c>
       <c r="X5" s="2">
         <v>1</v>
@@ -1114,8 +1199,11 @@
       <c r="Z5" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AB5" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>34</v>
       </c>
@@ -1134,8 +1222,11 @@
       <c r="F6" t="s">
         <v>70</v>
       </c>
-      <c r="V6" s="2">
-        <v>1</v>
+      <c r="G6" t="s">
+        <v>148</v>
+      </c>
+      <c r="H6" t="s">
+        <v>162</v>
       </c>
       <c r="X6" s="2">
         <v>1</v>
@@ -1143,8 +1234,11 @@
       <c r="Z6" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AB6" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>34</v>
       </c>
@@ -1163,18 +1257,21 @@
       <c r="F7" t="s">
         <v>71</v>
       </c>
-      <c r="O7" s="2"/>
-      <c r="V7" s="2">
-        <v>1</v>
-      </c>
+      <c r="H7" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q7" s="2"/>
       <c r="X7" s="2">
         <v>1</v>
       </c>
       <c r="Z7" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AB7" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>34</v>
       </c>
@@ -1193,19 +1290,25 @@
       <c r="F8" t="s">
         <v>72</v>
       </c>
-      <c r="P8" s="2"/>
-      <c r="Q8" s="2"/>
-      <c r="V8" s="2">
-        <v>1</v>
-      </c>
+      <c r="G8" t="s">
+        <v>149</v>
+      </c>
+      <c r="H8" t="s">
+        <v>162</v>
+      </c>
+      <c r="R8" s="2"/>
+      <c r="S8" s="2"/>
       <c r="X8" s="2">
         <v>1</v>
       </c>
       <c r="Z8" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AB8" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>34</v>
       </c>
@@ -1224,19 +1327,25 @@
       <c r="F9" t="s">
         <v>73</v>
       </c>
-      <c r="P9" s="2"/>
-      <c r="Q9" s="2"/>
-      <c r="V9" s="2">
-        <v>1</v>
-      </c>
+      <c r="G9" t="s">
+        <v>150</v>
+      </c>
+      <c r="H9" t="s">
+        <v>162</v>
+      </c>
+      <c r="R9" s="2"/>
+      <c r="S9" s="2"/>
       <c r="X9" s="2">
         <v>1</v>
       </c>
       <c r="Z9" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AB9" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>34</v>
       </c>
@@ -1255,18 +1364,24 @@
       <c r="F10" t="s">
         <v>74</v>
       </c>
-      <c r="S10" s="2"/>
-      <c r="V10" s="2">
-        <v>1</v>
-      </c>
+      <c r="G10" t="s">
+        <v>151</v>
+      </c>
+      <c r="H10" t="s">
+        <v>162</v>
+      </c>
+      <c r="U10" s="2"/>
       <c r="X10" s="2">
         <v>1</v>
       </c>
       <c r="Z10" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AB10" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>34</v>
       </c>
@@ -1285,18 +1400,24 @@
       <c r="F11" t="s">
         <v>75</v>
       </c>
-      <c r="T11" s="2"/>
-      <c r="V11" s="2">
-        <v>1</v>
-      </c>
+      <c r="G11" t="s">
+        <v>152</v>
+      </c>
+      <c r="H11" t="s">
+        <v>162</v>
+      </c>
+      <c r="V11" s="2"/>
       <c r="X11" s="2">
         <v>1</v>
       </c>
       <c r="Z11" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AB11" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>34</v>
       </c>
@@ -1315,8 +1436,11 @@
       <c r="F12" t="s">
         <v>76</v>
       </c>
-      <c r="V12" s="2">
-        <v>1</v>
+      <c r="G12" t="s">
+        <v>144</v>
+      </c>
+      <c r="H12" t="s">
+        <v>162</v>
       </c>
       <c r="X12" s="2">
         <v>1</v>
@@ -1324,8 +1448,11 @@
       <c r="Z12" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AB12" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>34</v>
       </c>
@@ -1344,8 +1471,11 @@
       <c r="F13" t="s">
         <v>77</v>
       </c>
-      <c r="V13" s="2">
-        <v>1</v>
+      <c r="G13" t="s">
+        <v>145</v>
+      </c>
+      <c r="H13" t="s">
+        <v>162</v>
       </c>
       <c r="X13" s="2">
         <v>1</v>
@@ -1353,8 +1483,11 @@
       <c r="Z13" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AB13" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>34</v>
       </c>
@@ -1373,8 +1506,11 @@
       <c r="F14" t="s">
         <v>78</v>
       </c>
-      <c r="V14" s="2">
-        <v>1</v>
+      <c r="G14" t="s">
+        <v>146</v>
+      </c>
+      <c r="H14" t="s">
+        <v>162</v>
       </c>
       <c r="X14" s="2">
         <v>1</v>
@@ -1382,8 +1518,11 @@
       <c r="Z14" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AB14" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>34</v>
       </c>
@@ -1402,8 +1541,12 @@
       <c r="F15" t="s">
         <v>79</v>
       </c>
-      <c r="V15" s="2">
-        <v>1</v>
+      <c r="G15" t="str">
+        <f t="shared" ref="G15:G66" si="0">B15&amp;"()"</f>
+        <v>industry()</v>
+      </c>
+      <c r="H15" t="s">
+        <v>10</v>
       </c>
       <c r="X15" s="2">
         <v>1</v>
@@ -1411,8 +1554,11 @@
       <c r="Z15" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AB15" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>34</v>
       </c>
@@ -1426,13 +1572,17 @@
         <v>34</v>
       </c>
       <c r="E16" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="F16" t="s">
         <v>80</v>
       </c>
-      <c r="V16" s="2">
-        <v>1</v>
+      <c r="G16" t="str">
+        <f t="shared" si="0"/>
+        <v>company_size()</v>
+      </c>
+      <c r="H16" t="s">
+        <v>155</v>
       </c>
       <c r="X16" s="2">
         <v>1</v>
@@ -1440,8 +1590,11 @@
       <c r="Z16" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AB16" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>34</v>
       </c>
@@ -1460,8 +1613,12 @@
       <c r="F17" t="s">
         <v>81</v>
       </c>
-      <c r="V17" s="2">
-        <v>1</v>
+      <c r="G17" t="str">
+        <f t="shared" si="0"/>
+        <v>annual_revenue()</v>
+      </c>
+      <c r="H17" t="s">
+        <v>155</v>
       </c>
       <c r="X17" s="2">
         <v>1</v>
@@ -1469,8 +1626,11 @@
       <c r="Z17" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AB17" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>34</v>
       </c>
@@ -1489,8 +1649,12 @@
       <c r="F18" t="s">
         <v>82</v>
       </c>
-      <c r="V18" s="2">
-        <v>1</v>
+      <c r="G18" t="str">
+        <f t="shared" si="0"/>
+        <v>tax_id()</v>
+      </c>
+      <c r="H18" t="s">
+        <v>155</v>
       </c>
       <c r="X18" s="2">
         <v>1</v>
@@ -1498,8 +1662,11 @@
       <c r="Z18" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AB18" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>34</v>
       </c>
@@ -1518,8 +1685,12 @@
       <c r="F19" t="s">
         <v>83</v>
       </c>
-      <c r="V19" s="2">
-        <v>1</v>
+      <c r="G19" t="str">
+        <f t="shared" si="0"/>
+        <v>registration_number()</v>
+      </c>
+      <c r="H19" t="s">
+        <v>155</v>
       </c>
       <c r="X19" s="2">
         <v>1</v>
@@ -1527,8 +1698,11 @@
       <c r="Z19" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AB19" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>34</v>
       </c>
@@ -1547,8 +1721,12 @@
       <c r="F20" t="s">
         <v>84</v>
       </c>
-      <c r="V20" s="2">
-        <v>1</v>
+      <c r="G20" t="str">
+        <f t="shared" si="0"/>
+        <v>payment_terms()</v>
+      </c>
+      <c r="H20" t="s">
+        <v>10</v>
       </c>
       <c r="X20" s="2">
         <v>1</v>
@@ -1556,8 +1734,11 @@
       <c r="Z20" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AB20" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>34</v>
       </c>
@@ -1576,8 +1757,12 @@
       <c r="F21" t="s">
         <v>85</v>
       </c>
-      <c r="V21" s="2">
-        <v>1</v>
+      <c r="G21" t="str">
+        <f t="shared" si="0"/>
+        <v>bank_name()</v>
+      </c>
+      <c r="H21" t="s">
+        <v>162</v>
       </c>
       <c r="X21" s="2">
         <v>1</v>
@@ -1585,8 +1770,11 @@
       <c r="Z21" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AB21" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>34</v>
       </c>
@@ -1605,8 +1793,12 @@
       <c r="F22" t="s">
         <v>86</v>
       </c>
-      <c r="V22" s="2">
-        <v>1</v>
+      <c r="G22" t="str">
+        <f t="shared" si="0"/>
+        <v>bank_account_number()</v>
+      </c>
+      <c r="H22" t="s">
+        <v>162</v>
       </c>
       <c r="X22" s="2">
         <v>1</v>
@@ -1614,8 +1806,11 @@
       <c r="Z22" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AB22" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>34</v>
       </c>
@@ -1634,8 +1829,12 @@
       <c r="F23" t="s">
         <v>87</v>
       </c>
-      <c r="V23" s="2">
-        <v>1</v>
+      <c r="G23" t="str">
+        <f t="shared" si="0"/>
+        <v>swift_code()</v>
+      </c>
+      <c r="H23" t="s">
+        <v>10</v>
       </c>
       <c r="X23" s="2">
         <v>1</v>
@@ -1643,8 +1842,11 @@
       <c r="Z23" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AB23" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>34</v>
       </c>
@@ -1663,8 +1865,12 @@
       <c r="F24" t="s">
         <v>99</v>
       </c>
-      <c r="V24" s="2">
-        <v>1</v>
+      <c r="G24" t="str">
+        <f t="shared" si="0"/>
+        <v>company_group()</v>
+      </c>
+      <c r="H24" t="s">
+        <v>10</v>
       </c>
       <c r="X24" s="2">
         <v>1</v>
@@ -1672,8 +1878,11 @@
       <c r="Z24" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AB24" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>34</v>
       </c>
@@ -1692,8 +1901,11 @@
       <c r="F25" t="s">
         <v>88</v>
       </c>
-      <c r="V25" s="2">
-        <v>1</v>
+      <c r="G25" t="s">
+        <v>143</v>
+      </c>
+      <c r="H25" t="s">
+        <v>162</v>
       </c>
       <c r="X25" s="2">
         <v>1</v>
@@ -1701,8 +1913,11 @@
       <c r="Z25" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AB25" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>34</v>
       </c>
@@ -1721,11 +1936,18 @@
       <c r="F26" t="s">
         <v>89</v>
       </c>
-      <c r="X26" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="G26" t="str">
+        <f t="shared" si="0"/>
+        <v>created_at()</v>
+      </c>
+      <c r="H26" t="s">
+        <v>157</v>
+      </c>
+      <c r="Z26" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>34</v>
       </c>
@@ -1744,31 +1966,45 @@
       <c r="F27" t="s">
         <v>90</v>
       </c>
-      <c r="X27" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="G27" t="str">
+        <f t="shared" si="0"/>
+        <v>updated_at()</v>
+      </c>
+      <c r="H27" t="s">
+        <v>157</v>
+      </c>
+      <c r="Z27" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>34</v>
       </c>
       <c r="B28" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="C28" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="D28" t="s">
         <v>34</v>
       </c>
       <c r="E28" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="F28" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.2">
+        <v>134</v>
+      </c>
+      <c r="G28" t="str">
+        <f t="shared" si="0"/>
+        <v>history()</v>
+      </c>
+      <c r="H28" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>34</v>
       </c>
@@ -1779,7 +2015,7 @@
         <v>91</v>
       </c>
       <c r="D29" t="s">
-        <v>100</v>
+        <v>142</v>
       </c>
       <c r="E29" t="s">
         <v>35</v>
@@ -1787,20 +2023,27 @@
       <c r="F29" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="V29" s="2">
-        <v>1</v>
-      </c>
-      <c r="W29">
-        <v>1</v>
+      <c r="G29" t="str">
+        <f t="shared" si="0"/>
+        <v>name()</v>
+      </c>
+      <c r="H29" t="s">
+        <v>162</v>
       </c>
       <c r="X29" s="2">
         <v>1</v>
       </c>
+      <c r="Y29">
+        <v>1</v>
+      </c>
       <c r="Z29" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AB29" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>34</v>
       </c>
@@ -1811,7 +2054,7 @@
         <v>92</v>
       </c>
       <c r="D30" t="s">
-        <v>100</v>
+        <v>142</v>
       </c>
       <c r="E30" t="s">
         <v>36</v>
@@ -1819,20 +2062,27 @@
       <c r="F30" t="s">
         <v>67</v>
       </c>
-      <c r="V30" s="2">
-        <v>1</v>
-      </c>
-      <c r="W30">
-        <v>1</v>
+      <c r="G30" t="str">
+        <f t="shared" si="0"/>
+        <v>email()</v>
+      </c>
+      <c r="H30" t="s">
+        <v>162</v>
       </c>
       <c r="X30" s="2">
         <v>1</v>
       </c>
+      <c r="Y30">
+        <v>1</v>
+      </c>
       <c r="Z30" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AB30" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>34</v>
       </c>
@@ -1843,7 +2093,7 @@
         <v>91</v>
       </c>
       <c r="D31" t="s">
-        <v>100</v>
+        <v>142</v>
       </c>
       <c r="E31" t="s">
         <v>37</v>
@@ -1851,8 +2101,12 @@
       <c r="F31" t="s">
         <v>68</v>
       </c>
-      <c r="V31" s="2">
-        <v>1</v>
+      <c r="G31" t="str">
+        <f t="shared" si="0"/>
+        <v>phone()</v>
+      </c>
+      <c r="H31" t="s">
+        <v>162</v>
       </c>
       <c r="X31" s="2">
         <v>1</v>
@@ -1860,8 +2114,11 @@
       <c r="Z31" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AB31" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>34</v>
       </c>
@@ -1872,7 +2129,7 @@
         <v>93</v>
       </c>
       <c r="D32" t="s">
-        <v>100</v>
+        <v>142</v>
       </c>
       <c r="E32" t="s">
         <v>39</v>
@@ -1880,8 +2137,11 @@
       <c r="F32" t="s">
         <v>69</v>
       </c>
-      <c r="V32" s="2">
-        <v>1</v>
+      <c r="G32" t="s">
+        <v>147</v>
+      </c>
+      <c r="H32" t="s">
+        <v>162</v>
       </c>
       <c r="X32" s="2">
         <v>1</v>
@@ -1889,8 +2149,11 @@
       <c r="Z32" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AB32" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>34</v>
       </c>
@@ -1901,7 +2164,7 @@
         <v>91</v>
       </c>
       <c r="D33" t="s">
-        <v>100</v>
+        <v>142</v>
       </c>
       <c r="E33" t="s">
         <v>41</v>
@@ -1909,8 +2172,11 @@
       <c r="F33" t="s">
         <v>70</v>
       </c>
-      <c r="V33" s="2">
-        <v>1</v>
+      <c r="G33" t="s">
+        <v>148</v>
+      </c>
+      <c r="H33" t="s">
+        <v>162</v>
       </c>
       <c r="X33" s="2">
         <v>1</v>
@@ -1918,8 +2184,11 @@
       <c r="Z33" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AB33" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>34</v>
       </c>
@@ -1930,7 +2199,7 @@
         <v>91</v>
       </c>
       <c r="D34" t="s">
-        <v>100</v>
+        <v>142</v>
       </c>
       <c r="E34" t="s">
         <v>41</v>
@@ -1938,8 +2207,12 @@
       <c r="F34" t="s">
         <v>71</v>
       </c>
-      <c r="V34" s="2">
-        <v>1</v>
+      <c r="G34" t="str">
+        <f t="shared" si="0"/>
+        <v>address_line_2()</v>
+      </c>
+      <c r="H34" t="s">
+        <v>10</v>
       </c>
       <c r="X34" s="2">
         <v>1</v>
@@ -1947,8 +2220,11 @@
       <c r="Z34" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AB34" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>34</v>
       </c>
@@ -1959,7 +2235,7 @@
         <v>91</v>
       </c>
       <c r="D35" t="s">
-        <v>100</v>
+        <v>142</v>
       </c>
       <c r="E35" t="s">
         <v>44</v>
@@ -1967,8 +2243,12 @@
       <c r="F35" t="s">
         <v>72</v>
       </c>
-      <c r="V35" s="2">
-        <v>1</v>
+      <c r="G35" t="str">
+        <f t="shared" si="0"/>
+        <v>city()</v>
+      </c>
+      <c r="H35" t="s">
+        <v>162</v>
       </c>
       <c r="X35" s="2">
         <v>1</v>
@@ -1976,8 +2256,11 @@
       <c r="Z35" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="36" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AB35" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>34</v>
       </c>
@@ -1988,7 +2271,7 @@
         <v>91</v>
       </c>
       <c r="D36" t="s">
-        <v>100</v>
+        <v>142</v>
       </c>
       <c r="E36" t="s">
         <v>44</v>
@@ -1996,8 +2279,12 @@
       <c r="F36" t="s">
         <v>73</v>
       </c>
-      <c r="V36" s="2">
-        <v>1</v>
+      <c r="G36" t="str">
+        <f t="shared" si="0"/>
+        <v>state()</v>
+      </c>
+      <c r="H36" t="s">
+        <v>162</v>
       </c>
       <c r="X36" s="2">
         <v>1</v>
@@ -2005,8 +2292,11 @@
       <c r="Z36" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AB36" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>34</v>
       </c>
@@ -2017,7 +2307,7 @@
         <v>91</v>
       </c>
       <c r="D37" t="s">
-        <v>100</v>
+        <v>142</v>
       </c>
       <c r="E37" t="s">
         <v>37</v>
@@ -2025,8 +2315,11 @@
       <c r="F37" t="s">
         <v>74</v>
       </c>
-      <c r="V37" s="2">
-        <v>1</v>
+      <c r="G37" t="s">
+        <v>151</v>
+      </c>
+      <c r="H37" t="s">
+        <v>162</v>
       </c>
       <c r="X37" s="2">
         <v>1</v>
@@ -2034,8 +2327,11 @@
       <c r="Z37" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="38" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AB37" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>34</v>
       </c>
@@ -2046,7 +2342,7 @@
         <v>91</v>
       </c>
       <c r="D38" t="s">
-        <v>100</v>
+        <v>142</v>
       </c>
       <c r="E38" t="s">
         <v>44</v>
@@ -2054,8 +2350,12 @@
       <c r="F38" t="s">
         <v>75</v>
       </c>
-      <c r="V38" s="2">
-        <v>1</v>
+      <c r="G38" t="str">
+        <f t="shared" si="0"/>
+        <v>country()</v>
+      </c>
+      <c r="H38" t="s">
+        <v>162</v>
       </c>
       <c r="X38" s="2">
         <v>1</v>
@@ -2063,8 +2363,11 @@
       <c r="Z38" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="39" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AB38" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>34</v>
       </c>
@@ -2075,7 +2378,7 @@
         <v>91</v>
       </c>
       <c r="D39" t="s">
-        <v>100</v>
+        <v>142</v>
       </c>
       <c r="E39" t="s">
         <v>44</v>
@@ -2083,8 +2386,11 @@
       <c r="F39" t="s">
         <v>76</v>
       </c>
-      <c r="V39" s="2">
-        <v>1</v>
+      <c r="G39" t="s">
+        <v>144</v>
+      </c>
+      <c r="H39" t="s">
+        <v>162</v>
       </c>
       <c r="X39" s="2">
         <v>1</v>
@@ -2092,8 +2398,11 @@
       <c r="Z39" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="40" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AB39" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>34</v>
       </c>
@@ -2104,7 +2413,7 @@
         <v>92</v>
       </c>
       <c r="D40" t="s">
-        <v>100</v>
+        <v>142</v>
       </c>
       <c r="E40" t="s">
         <v>36</v>
@@ -2112,8 +2421,11 @@
       <c r="F40" t="s">
         <v>77</v>
       </c>
-      <c r="V40" s="2">
-        <v>1</v>
+      <c r="G40" t="s">
+        <v>145</v>
+      </c>
+      <c r="H40" t="s">
+        <v>162</v>
       </c>
       <c r="X40" s="2">
         <v>1</v>
@@ -2121,8 +2433,11 @@
       <c r="Z40" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="41" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AB40" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>34</v>
       </c>
@@ -2133,7 +2448,7 @@
         <v>91</v>
       </c>
       <c r="D41" t="s">
-        <v>100</v>
+        <v>142</v>
       </c>
       <c r="E41" t="s">
         <v>37</v>
@@ -2141,8 +2456,11 @@
       <c r="F41" t="s">
         <v>78</v>
       </c>
-      <c r="V41" s="2">
-        <v>1</v>
+      <c r="G41" t="s">
+        <v>146</v>
+      </c>
+      <c r="H41" t="s">
+        <v>162</v>
       </c>
       <c r="X41" s="2">
         <v>1</v>
@@ -2150,8 +2468,11 @@
       <c r="Z41" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="42" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AB41" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>34</v>
       </c>
@@ -2162,7 +2483,7 @@
         <v>91</v>
       </c>
       <c r="D42" t="s">
-        <v>100</v>
+        <v>142</v>
       </c>
       <c r="E42" t="s">
         <v>44</v>
@@ -2170,8 +2491,12 @@
       <c r="F42" t="s">
         <v>79</v>
       </c>
-      <c r="V42" s="2">
-        <v>1</v>
+      <c r="G42" t="str">
+        <f t="shared" si="0"/>
+        <v>industry()</v>
+      </c>
+      <c r="H42" t="s">
+        <v>10</v>
       </c>
       <c r="X42" s="2">
         <v>1</v>
@@ -2179,8 +2504,11 @@
       <c r="Z42" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="43" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AB42" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>34</v>
       </c>
@@ -2191,16 +2519,20 @@
         <v>94</v>
       </c>
       <c r="D43" t="s">
-        <v>100</v>
+        <v>142</v>
       </c>
       <c r="E43" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="F43" t="s">
         <v>80</v>
       </c>
-      <c r="V43" s="2">
-        <v>1</v>
+      <c r="G43" t="str">
+        <f t="shared" si="0"/>
+        <v>company_size()</v>
+      </c>
+      <c r="H43" t="s">
+        <v>155</v>
       </c>
       <c r="X43" s="2">
         <v>1</v>
@@ -2208,8 +2540,11 @@
       <c r="Z43" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="44" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AB43" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>34</v>
       </c>
@@ -2220,7 +2555,7 @@
         <v>95</v>
       </c>
       <c r="D44" t="s">
-        <v>100</v>
+        <v>142</v>
       </c>
       <c r="E44" t="s">
         <v>54</v>
@@ -2228,8 +2563,12 @@
       <c r="F44" t="s">
         <v>81</v>
       </c>
-      <c r="V44" s="2">
-        <v>1</v>
+      <c r="G44" t="str">
+        <f t="shared" si="0"/>
+        <v>annual_revenue()</v>
+      </c>
+      <c r="H44" t="s">
+        <v>155</v>
       </c>
       <c r="X44" s="2">
         <v>1</v>
@@ -2237,8 +2576,11 @@
       <c r="Z44" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="45" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AB44" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>34</v>
       </c>
@@ -2249,7 +2591,7 @@
         <v>91</v>
       </c>
       <c r="D45" t="s">
-        <v>100</v>
+        <v>142</v>
       </c>
       <c r="E45" t="s">
         <v>56</v>
@@ -2257,8 +2599,11 @@
       <c r="F45" t="s">
         <v>82</v>
       </c>
-      <c r="V45" s="2">
-        <v>1</v>
+      <c r="G45" t="s">
+        <v>160</v>
+      </c>
+      <c r="H45" t="s">
+        <v>155</v>
       </c>
       <c r="X45" s="2">
         <v>1</v>
@@ -2266,8 +2611,11 @@
       <c r="Z45" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="46" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AB45" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>34</v>
       </c>
@@ -2278,7 +2626,7 @@
         <v>91</v>
       </c>
       <c r="D46" t="s">
-        <v>100</v>
+        <v>142</v>
       </c>
       <c r="E46" t="s">
         <v>56</v>
@@ -2286,8 +2634,11 @@
       <c r="F46" t="s">
         <v>83</v>
       </c>
-      <c r="V46" s="2">
-        <v>1</v>
+      <c r="G46" t="s">
+        <v>160</v>
+      </c>
+      <c r="H46" t="s">
+        <v>155</v>
       </c>
       <c r="X46" s="2">
         <v>1</v>
@@ -2295,8 +2646,11 @@
       <c r="Z46" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="47" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AB46" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>34</v>
       </c>
@@ -2307,7 +2661,7 @@
         <v>91</v>
       </c>
       <c r="D47" t="s">
-        <v>100</v>
+        <v>142</v>
       </c>
       <c r="E47" t="s">
         <v>44</v>
@@ -2315,8 +2669,8 @@
       <c r="F47" t="s">
         <v>84</v>
       </c>
-      <c r="V47" s="2">
-        <v>1</v>
+      <c r="H47" t="s">
+        <v>10</v>
       </c>
       <c r="X47" s="2">
         <v>1</v>
@@ -2324,8 +2678,11 @@
       <c r="Z47" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="48" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AB47" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>34</v>
       </c>
@@ -2336,7 +2693,7 @@
         <v>91</v>
       </c>
       <c r="D48" t="s">
-        <v>100</v>
+        <v>142</v>
       </c>
       <c r="E48" t="s">
         <v>44</v>
@@ -2344,8 +2701,12 @@
       <c r="F48" t="s">
         <v>85</v>
       </c>
-      <c r="V48" s="2">
-        <v>1</v>
+      <c r="G48" t="str">
+        <f t="shared" si="0"/>
+        <v>bank_name()</v>
+      </c>
+      <c r="H48" t="s">
+        <v>162</v>
       </c>
       <c r="X48" s="2">
         <v>1</v>
@@ -2353,8 +2714,11 @@
       <c r="Z48" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="49" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AB48" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>34</v>
       </c>
@@ -2365,7 +2729,7 @@
         <v>91</v>
       </c>
       <c r="D49" t="s">
-        <v>100</v>
+        <v>142</v>
       </c>
       <c r="E49" t="s">
         <v>56</v>
@@ -2373,8 +2737,12 @@
       <c r="F49" t="s">
         <v>86</v>
       </c>
-      <c r="V49" s="2">
-        <v>1</v>
+      <c r="G49" t="str">
+        <f t="shared" si="0"/>
+        <v>bank_account_number()</v>
+      </c>
+      <c r="H49" t="s">
+        <v>162</v>
       </c>
       <c r="X49" s="2">
         <v>1</v>
@@ -2382,8 +2750,11 @@
       <c r="Z49" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="50" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AB49" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>34</v>
       </c>
@@ -2394,7 +2765,7 @@
         <v>91</v>
       </c>
       <c r="D50" t="s">
-        <v>100</v>
+        <v>142</v>
       </c>
       <c r="E50" t="s">
         <v>56</v>
@@ -2402,8 +2773,8 @@
       <c r="F50" t="s">
         <v>87</v>
       </c>
-      <c r="V50" s="2">
-        <v>1</v>
+      <c r="H50" t="s">
+        <v>10</v>
       </c>
       <c r="X50" s="2">
         <v>1</v>
@@ -2411,8 +2782,11 @@
       <c r="Z50" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="51" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AB50" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>34</v>
       </c>
@@ -2423,7 +2797,7 @@
         <v>91</v>
       </c>
       <c r="D51" t="s">
-        <v>100</v>
+        <v>142</v>
       </c>
       <c r="E51" t="s">
         <v>44</v>
@@ -2431,8 +2805,8 @@
       <c r="F51" t="s">
         <v>99</v>
       </c>
-      <c r="V51" s="2">
-        <v>1</v>
+      <c r="H51" t="s">
+        <v>10</v>
       </c>
       <c r="X51" s="2">
         <v>1</v>
@@ -2440,8 +2814,11 @@
       <c r="Z51" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="52" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AB51" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>34</v>
       </c>
@@ -2452,7 +2829,7 @@
         <v>96</v>
       </c>
       <c r="D52" t="s">
-        <v>100</v>
+        <v>142</v>
       </c>
       <c r="E52" t="s">
         <v>63</v>
@@ -2460,8 +2837,11 @@
       <c r="F52" t="s">
         <v>88</v>
       </c>
-      <c r="V52" s="2">
-        <v>1</v>
+      <c r="G52" t="s">
+        <v>143</v>
+      </c>
+      <c r="H52" t="s">
+        <v>162</v>
       </c>
       <c r="X52" s="2">
         <v>1</v>
@@ -2469,8 +2849,11 @@
       <c r="Z52" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="53" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AB52" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>34</v>
       </c>
@@ -2481,7 +2864,7 @@
         <v>97</v>
       </c>
       <c r="D53" t="s">
-        <v>100</v>
+        <v>142</v>
       </c>
       <c r="E53" t="s">
         <v>64</v>
@@ -2489,11 +2872,18 @@
       <c r="F53" t="s">
         <v>89</v>
       </c>
-      <c r="X53" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="G53" t="str">
+        <f t="shared" si="0"/>
+        <v>created_at()</v>
+      </c>
+      <c r="H53" t="s">
+        <v>157</v>
+      </c>
+      <c r="Z53" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>34</v>
       </c>
@@ -2504,7 +2894,7 @@
         <v>97</v>
       </c>
       <c r="D54" t="s">
-        <v>100</v>
+        <v>142</v>
       </c>
       <c r="E54" t="s">
         <v>65</v>
@@ -2512,36 +2902,50 @@
       <c r="F54" t="s">
         <v>90</v>
       </c>
-      <c r="X54" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="G54" t="str">
+        <f t="shared" si="0"/>
+        <v>updated_at()</v>
+      </c>
+      <c r="H54" t="s">
+        <v>157</v>
+      </c>
+      <c r="Z54" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>34</v>
       </c>
       <c r="B55" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="C55" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="D55" t="s">
-        <v>100</v>
+        <v>142</v>
       </c>
       <c r="E55" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="F55" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="56" spans="1:26" x14ac:dyDescent="0.2">
+        <v>134</v>
+      </c>
+      <c r="G55" t="str">
+        <f t="shared" si="0"/>
+        <v>history()</v>
+      </c>
+      <c r="H55" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="56" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>34</v>
       </c>
       <c r="B56" t="s">
-        <v>102</v>
+        <v>47</v>
       </c>
       <c r="C56" t="s">
         <v>91</v>
@@ -2555,25 +2959,29 @@
       <c r="F56" t="s">
         <v>75</v>
       </c>
-      <c r="V56" s="2">
-        <v>1</v>
-      </c>
-      <c r="W56">
-        <v>1</v>
+      <c r="G56" t="str">
+        <f t="shared" si="0"/>
+        <v>country()</v>
       </c>
       <c r="X56" s="2">
         <v>1</v>
       </c>
+      <c r="Y56">
+        <v>1</v>
+      </c>
       <c r="Z56" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="57" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AB56" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>34</v>
       </c>
       <c r="B57" t="s">
-        <v>103</v>
+        <v>138</v>
       </c>
       <c r="C57" t="s">
         <v>91</v>
@@ -2582,13 +2990,13 @@
         <v>101</v>
       </c>
       <c r="E57" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="F57" t="s">
-        <v>111</v>
-      </c>
-      <c r="V57" s="2">
-        <v>1</v>
+        <v>106</v>
+      </c>
+      <c r="H57" t="s">
+        <v>155</v>
       </c>
       <c r="X57" s="2">
         <v>1</v>
@@ -2596,13 +3004,16 @@
       <c r="Z57" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="58" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AB57" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>34</v>
       </c>
       <c r="B58" t="s">
-        <v>104</v>
+        <v>139</v>
       </c>
       <c r="C58" t="s">
         <v>95</v>
@@ -2611,13 +3022,13 @@
         <v>101</v>
       </c>
       <c r="E58" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="F58" t="s">
-        <v>112</v>
-      </c>
-      <c r="V58" s="2">
-        <v>1</v>
+        <v>107</v>
+      </c>
+      <c r="H58" t="s">
+        <v>156</v>
       </c>
       <c r="X58" s="2">
         <v>1</v>
@@ -2625,28 +3036,31 @@
       <c r="Z58" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="59" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AB58" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>34</v>
       </c>
       <c r="B59" t="s">
+        <v>140</v>
+      </c>
+      <c r="C59" t="s">
         <v>105</v>
-      </c>
-      <c r="C59" t="s">
-        <v>110</v>
       </c>
       <c r="D59" t="s">
         <v>101</v>
       </c>
       <c r="E59" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="F59" t="s">
-        <v>113</v>
-      </c>
-      <c r="V59" s="2">
-        <v>1</v>
+        <v>108</v>
+      </c>
+      <c r="H59" t="s">
+        <v>10</v>
       </c>
       <c r="X59" s="2">
         <v>1</v>
@@ -2654,13 +3068,16 @@
       <c r="Z59" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="60" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AB59" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>34</v>
       </c>
       <c r="B60" t="s">
-        <v>106</v>
+        <v>141</v>
       </c>
       <c r="C60" t="s">
         <v>94</v>
@@ -2669,13 +3086,13 @@
         <v>101</v>
       </c>
       <c r="E60" t="s">
+        <v>104</v>
+      </c>
+      <c r="F60" t="s">
         <v>109</v>
       </c>
-      <c r="F60" t="s">
-        <v>114</v>
-      </c>
-      <c r="V60" s="2">
-        <v>1</v>
+      <c r="H60" t="s">
+        <v>155</v>
       </c>
       <c r="X60" s="2">
         <v>1</v>
@@ -2683,28 +3100,35 @@
       <c r="Z60" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="61" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AB60" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>34</v>
       </c>
       <c r="B61" t="s">
+        <v>111</v>
+      </c>
+      <c r="C61" t="s">
+        <v>112</v>
+      </c>
+      <c r="D61" t="s">
+        <v>135</v>
+      </c>
+      <c r="E61" t="s">
         <v>116</v>
       </c>
-      <c r="C61" t="s">
-        <v>117</v>
-      </c>
-      <c r="D61" t="s">
-        <v>141</v>
-      </c>
-      <c r="E61" t="s">
+      <c r="F61" t="s">
         <v>122</v>
       </c>
-      <c r="F61" t="s">
-        <v>128</v>
-      </c>
-      <c r="V61" s="2">
-        <v>1</v>
+      <c r="G61" t="str">
+        <f t="shared" si="0"/>
+        <v>company()</v>
+      </c>
+      <c r="H61" t="s">
+        <v>162</v>
       </c>
       <c r="X61" s="2">
         <v>1</v>
@@ -2712,28 +3136,34 @@
       <c r="Z61" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="62" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AB61" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>34</v>
       </c>
       <c r="B62" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="C62" t="s">
         <v>91</v>
       </c>
       <c r="D62" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="E62" t="s">
         <v>35</v>
       </c>
       <c r="F62" t="s">
-        <v>131</v>
-      </c>
-      <c r="V62" s="2">
-        <v>1</v>
+        <v>125</v>
+      </c>
+      <c r="G62" t="s">
+        <v>153</v>
+      </c>
+      <c r="H62" t="s">
+        <v>162</v>
       </c>
       <c r="X62" s="2">
         <v>1</v>
@@ -2741,28 +3171,35 @@
       <c r="Z62" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="63" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AB62" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>34</v>
       </c>
       <c r="B63" t="s">
-        <v>119</v>
+        <v>158</v>
       </c>
       <c r="C63" t="s">
         <v>91</v>
       </c>
       <c r="D63" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="E63" t="s">
         <v>35</v>
       </c>
       <c r="F63" t="s">
-        <v>127</v>
-      </c>
-      <c r="V63" s="2">
-        <v>1</v>
+        <v>121</v>
+      </c>
+      <c r="G63" t="str">
+        <f>B63&amp;"()"</f>
+        <v>first_name()</v>
+      </c>
+      <c r="H63" t="s">
+        <v>162</v>
       </c>
       <c r="X63" s="2">
         <v>1</v>
@@ -2770,28 +3207,34 @@
       <c r="Z63" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="64" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AB63" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>34</v>
       </c>
       <c r="B64" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="C64" t="s">
         <v>91</v>
       </c>
       <c r="D64" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="E64" t="s">
         <v>35</v>
       </c>
       <c r="F64" t="s">
-        <v>126</v>
-      </c>
-      <c r="V64" s="2">
-        <v>1</v>
+        <v>120</v>
+      </c>
+      <c r="G64" t="s">
+        <v>159</v>
+      </c>
+      <c r="H64" t="s">
+        <v>162</v>
       </c>
       <c r="X64" s="2">
         <v>1</v>
@@ -2799,8 +3242,11 @@
       <c r="Z64" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="65" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AB64" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>34</v>
       </c>
@@ -2811,16 +3257,20 @@
         <v>92</v>
       </c>
       <c r="D65" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="E65" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="F65" t="s">
         <v>31</v>
       </c>
-      <c r="V65" s="2">
-        <v>1</v>
+      <c r="G65" t="str">
+        <f t="shared" si="0"/>
+        <v>email()</v>
+      </c>
+      <c r="H65" t="s">
+        <v>162</v>
       </c>
       <c r="X65" s="2">
         <v>1</v>
@@ -2828,8 +3278,11 @@
       <c r="Z65" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="66" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AB65" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>34</v>
       </c>
@@ -2840,16 +3293,20 @@
         <v>91</v>
       </c>
       <c r="D66" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="E66" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="F66" t="s">
         <v>32</v>
       </c>
-      <c r="V66" s="2">
-        <v>1</v>
+      <c r="G66" t="str">
+        <f t="shared" si="0"/>
+        <v>phone()</v>
+      </c>
+      <c r="H66" t="s">
+        <v>162</v>
       </c>
       <c r="X66" s="2">
         <v>1</v>
@@ -2857,28 +3314,34 @@
       <c r="Z66" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="67" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AB66" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>34</v>
       </c>
       <c r="B67" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="C67" t="s">
         <v>91</v>
       </c>
       <c r="D67" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="E67" t="s">
+        <v>117</v>
+      </c>
+      <c r="F67" t="s">
         <v>123</v>
       </c>
-      <c r="F67" t="s">
-        <v>129</v>
-      </c>
-      <c r="V67" s="2">
-        <v>1</v>
+      <c r="G67" t="s">
+        <v>143</v>
+      </c>
+      <c r="H67" t="s">
+        <v>162</v>
       </c>
       <c r="X67" s="2">
         <v>1</v>
@@ -2886,28 +3349,34 @@
       <c r="Z67" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="68" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AB67" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>34</v>
       </c>
       <c r="B68" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="C68" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="D68" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="E68" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="F68" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="69" spans="1:26" x14ac:dyDescent="0.2">
+        <v>134</v>
+      </c>
+      <c r="H68" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="69" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>34</v>
       </c>
@@ -2918,7 +3387,7 @@
         <v>97</v>
       </c>
       <c r="D69" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="E69" t="s">
         <v>64</v>
@@ -2926,11 +3395,14 @@
       <c r="F69" t="s">
         <v>89</v>
       </c>
-      <c r="X69" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="70" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="H69" t="s">
+        <v>157</v>
+      </c>
+      <c r="Z69" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>34</v>
       </c>
@@ -2941,7 +3413,7 @@
         <v>97</v>
       </c>
       <c r="D70" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="E70" t="s">
         <v>65</v>
@@ -2949,7 +3421,10 @@
       <c r="F70" t="s">
         <v>90</v>
       </c>
-      <c r="X70" s="2">
+      <c r="H70" t="s">
+        <v>157</v>
+      </c>
+      <c r="Z70" s="2">
         <v>1</v>
       </c>
     </row>
@@ -2971,7 +3446,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="B1" t="s">
         <v>33</v>
@@ -2997,7 +3472,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="B1" t="s">
         <v>33</v>
@@ -3023,7 +3498,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>33</v>
@@ -3049,7 +3524,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>33</v>
@@ -3075,7 +3550,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>33</v>
@@ -3105,7 +3580,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="B1" t="s">
         <v>33</v>
@@ -3133,7 +3608,7 @@
         <v>34</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -3155,7 +3630,7 @@
         <v>100</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -3166,7 +3641,7 @@
         <v>101</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -3174,10 +3649,10 @@
         <v>34</v>
       </c>
       <c r="B7" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="51" x14ac:dyDescent="0.2">
@@ -3185,10 +3660,10 @@
         <v>34</v>
       </c>
       <c r="B8" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -3201,7 +3676,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3211,7 +3686,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="B1" t="s">
         <v>33</v>
@@ -3228,7 +3703,7 @@
         <v>34</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -3252,7 +3727,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="B1" t="s">
         <v>33</v>
@@ -3281,7 +3756,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="B1" t="s">
         <v>33</v>
@@ -3307,7 +3782,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="B1" t="s">
         <v>33</v>

</xml_diff>